<commit_message>
CoilDesign\\DEXTER_WORKSPACE\\CAD stuff\\Final_CAD: Reverted back to the original plan, all parameters are controlled by an excel file --- Can't check this --- Inventor hates Onedrive :(
</commit_message>
<xml_diff>
--- a/CoilDesign/DEXTER_WORKSPACE/CAD stuff/Final_CAD/parameters.xlsx
+++ b/CoilDesign/DEXTER_WORKSPACE/CAD stuff/Final_CAD/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SUMMER 2020\oldGitRevert\2020-srw-rc-car\CoilDesign\DEXTER_WORKSPACE\CAD stuff\Final_CAD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52957697aad046c3/UoA/2020 SUMMER/2020-srw-rc-car/CoilDesign/DEXTER_WORKSPACE/CAD stuff/Final_CAD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B894CE7C-1470-445E-B95F-B87383C43091}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{B894CE7C-1470-445E-B95F-B87383C43091}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{60A83059-FEE4-4DD6-B332-D4F16B4CAEC4}"/>
   <bookViews>
-    <workbookView xWindow="5535" yWindow="5355" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -514,7 +514,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
CoilDesign\\DEXTER_WORKSPACE\\CAD stuff\\Final_CAD\\Adobe_Illustrator: Added UoA vector logo --- not sure if I made it right???
</commit_message>
<xml_diff>
--- a/CoilDesign/DEXTER_WORKSPACE/CAD stuff/Final_CAD/parameters.xlsx
+++ b/CoilDesign/DEXTER_WORKSPACE/CAD stuff/Final_CAD/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52957697aad046c3/UoA/2020 SUMMER/2020-srw-rc-car/CoilDesign/DEXTER_WORKSPACE/CAD stuff/Final_CAD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SUMMER 2020\oldGitRevert\2020-srw-rc-car\CoilDesign\DEXTER_WORKSPACE\CAD stuff\Final_CAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{B894CE7C-1470-445E-B95F-B87383C43091}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{60A83059-FEE4-4DD6-B332-D4F16B4CAEC4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C331D750-6821-4DEC-BC5F-CA62FA25C89E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>track_length</t>
   </si>
@@ -169,20 +169,22 @@
   </si>
   <si>
     <t>Equation</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -227,10 +229,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,22 +522,23 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.5703125" customWidth="1"/>
+    <col min="2" max="2" width="73.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>45</v>
       </c>
     </row>
@@ -601,8 +610,8 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>49</v>
+      <c r="B10" s="4">
+        <v>7</v>
       </c>
       <c r="C10" t="s">
         <v>44</v>
@@ -652,8 +661,8 @@
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>48</v>
+      <c r="B16" s="4">
+        <v>5</v>
       </c>
       <c r="C16" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
CoilDesign\\DEXTER_WORKSPACE\\CAD stuff\\Final_CAD\\ some where in my folder idk: Updated ferrite_layer with the correct dimensions, fixed dimensions in the excel file, added some Engraving templates .ai
</commit_message>
<xml_diff>
--- a/CoilDesign/DEXTER_WORKSPACE/CAD stuff/Final_CAD/parameters.xlsx
+++ b/CoilDesign/DEXTER_WORKSPACE/CAD stuff/Final_CAD/parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\files.auckland.ac.nz\myhome\Documents\GitHub\2020-srw-rc-car\CoilDesign\DEXTER_WORKSPACE\CAD stuff\Final_CAD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\files.auckland.ac.nz\myhome\SUMMER 2020\oldGitRevert\2020-srw-rc-car\CoilDesign\DEXTER_WORKSPACE\CAD stuff\Final_CAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B38C626-6225-406F-A15C-7879A3FF4724}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E50364-9EE0-42F3-A0DF-C203BA1B259F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,9 +114,6 @@
     <t>500 mm</t>
   </si>
   <si>
-    <t>109 mm</t>
-  </si>
-  <si>
     <t>15 mm</t>
   </si>
   <si>
@@ -169,6 +166,9 @@
   </si>
   <si>
     <t>75 mm</t>
+  </si>
+  <si>
+    <t>218 mm</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,13 +533,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -587,7 +587,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -595,7 +595,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -603,7 +603,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -614,7 +614,7 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -622,7 +622,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -630,7 +630,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -638,7 +638,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -646,7 +646,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -654,7 +654,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -665,7 +665,7 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -673,7 +673,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -681,7 +681,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -697,7 +697,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -705,7 +705,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -713,7 +713,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -721,7 +721,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -737,7 +737,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -745,7 +745,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>